<commit_message>
Add new stat sheet
</commit_message>
<xml_diff>
--- a/Redis cli benchmark.xlsx
+++ b/Redis cli benchmark.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Pipeline size" sheetId="1" r:id="rId1"/>
+    <sheet name="Hashmap size" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t>credis_bench</t>
   </si>
@@ -184,25 +185,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.624448537826538</c:v>
+                  <c:v>2.18760681152344</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.196943283081055</c:v>
+                  <c:v>4.03100562095642</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.049156188964844</c:v>
+                  <c:v>5.81422090530396</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.919826745986938</c:v>
+                  <c:v>1.93569707870483</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.936469793319702</c:v>
+                  <c:v>6.79749774932861</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.892753839492798</c:v>
+                  <c:v>1.90157675743103</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.874435901641846</c:v>
+                  <c:v>1.95318412780762</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -264,25 +265,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.472078561782837</c:v>
+                  <c:v>2.69019603729248</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.448967933654785</c:v>
+                  <c:v>5.72161102294922</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4697425365448</c:v>
+                  <c:v>5.08827948570251</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.48812460899353</c:v>
+                  <c:v>2.64856791496277</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.512061834335327</c:v>
+                  <c:v>4.19528150558472</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.444071292877197</c:v>
+                  <c:v>2.60411190986633</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.417610883712769</c:v>
+                  <c:v>2.45635485649109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -344,25 +345,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4.40124249458313</c:v>
+                  <c:v>5.39368796348572</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.815352201461792</c:v>
+                  <c:v>6.98980760574341</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.75149941444397</c:v>
+                  <c:v>10.3803336620331</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.544238805770874</c:v>
+                  <c:v>8.58077549934387</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.774335622787476</c:v>
+                  <c:v>8.06004762649536</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.440513372421265</c:v>
+                  <c:v>3.47025609016418</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.480040073394775</c:v>
+                  <c:v>3.52133131027222</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -424,25 +425,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>8.978171110153198</c:v>
+                  <c:v>29.784951210022</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.055680990219116</c:v>
+                  <c:v>16.1310484409332</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.762266159057617</c:v>
+                  <c:v>22.753564119339</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.477071046829224</c:v>
+                  <c:v>24.4482481479645</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.522807598114014</c:v>
+                  <c:v>8.9083616733551</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.640124797821045</c:v>
+                  <c:v>8.64669179916382</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.403800964355469</c:v>
+                  <c:v>16.1964256763458</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -529,7 +530,452 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hashmap size'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>credis_bench</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="E41A1C"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Hashmap size'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Hashmap size'!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.00534796714782715</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0201034545898438</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0326426029205322</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.189861536026001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.404411554336548</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.03817319869995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.03708648681641</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hashmap size'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pipelayer_bench</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="377EB8"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Hashmap size'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Hashmap size'!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.00516557693481445</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0276470184326172</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0533850193023682</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.309478759765625</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.549838542938232</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.96565556526184</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.91912722587585</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hashmap size'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pipelayerlib_bench</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4DAF4A"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Hashmap size'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Hashmap size'!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.00696611404418945</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.043175220489502</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0637373924255371</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.443438053131104</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.709036111831665</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.07474446296692</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.45492315292358</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Hashmap size'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>redispy_bench</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="984EA3"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Hashmap size'!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Hashmap size'!$E$2:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.0183093547821045</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.106787443161011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.175554513931274</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.979166030883789</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.80770707130432</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.5105519294739</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16.178120136261</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:overlap val="-10"/>
+        <c:axId val="50020001"/>
+        <c:axId val="50020002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50020001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Pipeline size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50020002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -874,16 +1320,16 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>2.624448537826538</v>
+        <v>2.18760681152344</v>
       </c>
       <c r="C2">
-        <v>2.472078561782837</v>
+        <v>2.69019603729248</v>
       </c>
       <c r="D2">
-        <v>4.40124249458313</v>
+        <v>5.39368796348572</v>
       </c>
       <c r="E2">
-        <v>8.978171110153198</v>
+        <v>29.784951210022</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -891,16 +1337,16 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>2.196943283081055</v>
+        <v>4.03100562095642</v>
       </c>
       <c r="C3">
-        <v>2.448967933654785</v>
+        <v>5.72161102294922</v>
       </c>
       <c r="D3">
-        <v>3.815352201461792</v>
+        <v>6.98980760574341</v>
       </c>
       <c r="E3">
-        <v>9.055680990219116</v>
+        <v>16.1310484409332</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -908,16 +1354,16 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>2.049156188964844</v>
+        <v>5.81422090530396</v>
       </c>
       <c r="C4">
-        <v>2.4697425365448</v>
+        <v>5.08827948570251</v>
       </c>
       <c r="D4">
-        <v>3.75149941444397</v>
+        <v>10.3803336620331</v>
       </c>
       <c r="E4">
-        <v>8.762266159057617</v>
+        <v>22.753564119339</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -925,16 +1371,16 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>1.919826745986938</v>
+        <v>1.93569707870483</v>
       </c>
       <c r="C5">
-        <v>2.48812460899353</v>
+        <v>2.64856791496277</v>
       </c>
       <c r="D5">
-        <v>3.544238805770874</v>
+        <v>8.58077549934387</v>
       </c>
       <c r="E5">
-        <v>8.477071046829224</v>
+        <v>24.4482481479645</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -942,16 +1388,16 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>1.936469793319702</v>
+        <v>6.79749774932861</v>
       </c>
       <c r="C6">
-        <v>2.512061834335327</v>
+        <v>4.19528150558472</v>
       </c>
       <c r="D6">
-        <v>3.774335622787476</v>
+        <v>8.06004762649536</v>
       </c>
       <c r="E6">
-        <v>8.522807598114014</v>
+        <v>8.9083616733551</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -959,16 +1405,16 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>1.892753839492798</v>
+        <v>1.90157675743103</v>
       </c>
       <c r="C7">
-        <v>2.444071292877197</v>
+        <v>2.60411190986633</v>
       </c>
       <c r="D7">
-        <v>3.440513372421265</v>
+        <v>3.47025609016418</v>
       </c>
       <c r="E7">
-        <v>8.640124797821045</v>
+        <v>8.64669179916382</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -976,16 +1422,163 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>1.874435901641846</v>
+        <v>1.95318412780762</v>
       </c>
       <c r="C8">
-        <v>2.417610883712769</v>
+        <v>2.45635485649109</v>
       </c>
       <c r="D8">
-        <v>3.480040073394775</v>
+        <v>3.52133131027222</v>
       </c>
       <c r="E8">
-        <v>8.403800964355469</v>
+        <v>16.1964256763458</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>0.00534796714782715</v>
+      </c>
+      <c r="C2">
+        <v>0.00516557693481445</v>
+      </c>
+      <c r="D2">
+        <v>0.00696611404418945</v>
+      </c>
+      <c r="E2">
+        <v>0.0183093547821045</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>0.0201034545898438</v>
+      </c>
+      <c r="C3">
+        <v>0.0276470184326172</v>
+      </c>
+      <c r="D3">
+        <v>0.043175220489502</v>
+      </c>
+      <c r="E3">
+        <v>0.106787443161011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>0.0326426029205322</v>
+      </c>
+      <c r="C4">
+        <v>0.0533850193023682</v>
+      </c>
+      <c r="D4">
+        <v>0.0637373924255371</v>
+      </c>
+      <c r="E4">
+        <v>0.175554513931274</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>0.189861536026001</v>
+      </c>
+      <c r="C5">
+        <v>0.309478759765625</v>
+      </c>
+      <c r="D5">
+        <v>0.443438053131104</v>
+      </c>
+      <c r="E5">
+        <v>0.979166030883789</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>0.404411554336548</v>
+      </c>
+      <c r="C6">
+        <v>0.549838542938232</v>
+      </c>
+      <c r="D6">
+        <v>0.709036111831665</v>
+      </c>
+      <c r="E6">
+        <v>1.80770707130432</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>2.03817319869995</v>
+      </c>
+      <c r="C7">
+        <v>2.96565556526184</v>
+      </c>
+      <c r="D7">
+        <v>4.07474446296692</v>
+      </c>
+      <c r="E7">
+        <v>15.5105519294739</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>4.03708648681641</v>
+      </c>
+      <c r="C8">
+        <v>7.91912722587585</v>
+      </c>
+      <c r="D8">
+        <v>6.45492315292358</v>
+      </c>
+      <c r="E8">
+        <v>16.178120136261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>